<commit_message>
Data retrieval and visual presentation.
</commit_message>
<xml_diff>
--- a/db/Data.xlsx
+++ b/db/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DotNet\thesis-engineering-exercise\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15870A65-CC90-4CA5-BC8A-5BBFDB542E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFA8E25-419E-4935-90B0-6125B89F739D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2C05AAD8-FCEC-4ED1-8319-B8E86917EE04}"/>
   </bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>